<commit_message>
Add video link for Thierry Boisivon 4x4x4
</commit_message>
<xml_diff>
--- a/data/2020-02-25/Senior Cubers Worldwide - Weekly Competition - 2020-02-25.xlsx
+++ b/data/2020-02-25/Senior Cubers Worldwide - Weekly Competition - 2020-02-25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-02-25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B56D3440-ACC5-498B-9E0C-DC681858FEA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEC6CEE-7E1D-416A-A2FE-DB7872A21FF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3x3x3" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="FMC" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -390,9 +389,6 @@
     <t>1:26.27</t>
   </si>
   <si>
-    <t>will load video on Monday</t>
-  </si>
-  <si>
     <t>Aaron Cumes</t>
   </si>
   <si>
@@ -659,12 +655,15 @@
   <si>
     <t>🥉</t>
   </si>
+  <si>
+    <t>https://www.facebook.com/events/805797596592397/permalink/810222906149866/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -774,6 +773,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -798,10 +803,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -932,8 +938,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1152,8 +1160,8 @@
   </sheetPr>
   <dimension ref="A1:L1059"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1239,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>18</v>
@@ -1248,7 +1256,7 @@
         <v>13.73</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F4" s="19">
         <v>15.99</v>
@@ -1316,7 +1324,7 @@
         <v>14.53</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F6" s="19">
         <v>14.55</v>
@@ -1351,7 +1359,7 @@
         <v>15.64</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F7" s="19">
         <v>14.75</v>
@@ -1386,7 +1394,7 @@
         <v>18.48</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F8" s="19">
         <v>18.55</v>
@@ -1676,7 +1684,7 @@
         <v>19.77</v>
       </c>
       <c r="K16" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="12.75">
@@ -1684,7 +1692,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>19</v>
@@ -1708,7 +1716,7 @@
         <v>21.96</v>
       </c>
       <c r="K17" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="12.75">
@@ -1716,7 +1724,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C18" s="30" t="s">
         <v>18</v>
@@ -1740,7 +1748,7 @@
         <v>24.61</v>
       </c>
       <c r="K18" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="12.75">
@@ -1748,7 +1756,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>19</v>
@@ -1772,7 +1780,7 @@
         <v>23.6</v>
       </c>
       <c r="K19" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="12.75">
@@ -1807,7 +1815,7 @@
         <v>24</v>
       </c>
       <c r="K20" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="12.75">
@@ -1815,7 +1823,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>19</v>
@@ -1839,7 +1847,7 @@
         <v>26.02</v>
       </c>
       <c r="K21" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="12.75">
@@ -1847,7 +1855,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>19</v>
@@ -1871,7 +1879,7 @@
         <v>27.27</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="12.75">
@@ -1906,7 +1914,7 @@
         <v>27.3</v>
       </c>
       <c r="K23" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="12.75">
@@ -1914,7 +1922,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C24" s="36" t="s">
         <v>19</v>
@@ -1941,7 +1949,7 @@
         <v>31.57</v>
       </c>
       <c r="K24" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="12.75">
@@ -1949,7 +1957,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C25" s="36" t="s">
         <v>35</v>
@@ -1973,7 +1981,7 @@
         <v>32.08</v>
       </c>
       <c r="K25" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="12.75">
@@ -1981,7 +1989,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>35</v>
@@ -2005,7 +2013,7 @@
         <v>37.72</v>
       </c>
       <c r="K26" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="12.75">
@@ -2013,13 +2021,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>30</v>
@@ -2034,13 +2042,13 @@
         <v>39.49</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>24</v>
       </c>
       <c r="K27" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="12.75">
@@ -13431,7 +13439,7 @@
   <dimension ref="A1:L1039"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A4" sqref="A4:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -13517,7 +13525,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>18</v>
@@ -13526,7 +13534,7 @@
         <v>4.55</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F4" s="19">
         <v>4.6900000000000004</v>
@@ -13561,7 +13569,7 @@
         <v>5.08</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F5" s="19">
         <v>5.96</v>
@@ -13596,7 +13604,7 @@
         <v>5.17</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F6" s="19">
         <v>4.6399999999999997</v>
@@ -13663,7 +13671,7 @@
         <v>5.83</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F8" s="19">
         <v>5.09</v>
@@ -13894,7 +13902,7 @@
         <v>4.83</v>
       </c>
       <c r="K14" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="12.75">
@@ -13927,7 +13935,7 @@
         <v>10.85</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12.75">
@@ -13935,7 +13943,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C16" s="31" t="s">
         <v>19</v>
@@ -13962,7 +13970,7 @@
         <v>4.76</v>
       </c>
       <c r="K16" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="12.75">
@@ -13970,7 +13978,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>19</v>
@@ -13994,7 +14002,7 @@
         <v>9.85</v>
       </c>
       <c r="K17" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="12.75">
@@ -14002,7 +14010,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C18" s="31" t="s">
         <v>19</v>
@@ -14029,7 +14037,7 @@
         <v>11.32</v>
       </c>
       <c r="K18" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="12.75">
@@ -14037,7 +14045,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>35</v>
@@ -14061,7 +14069,7 @@
         <v>13.71</v>
       </c>
       <c r="K19" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="12.75">
@@ -14069,7 +14077,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C20" s="31" t="s">
         <v>19</v>
@@ -14096,7 +14104,7 @@
         <v>16.28</v>
       </c>
       <c r="K20" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="12.75">
@@ -20481,6 +20489,7 @@
     <hyperlink ref="K20" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -20492,7 +20501,7 @@
   <dimension ref="A1:L1038"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -20587,7 +20596,7 @@
         <v>53.3</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F4" s="17">
         <v>48.44</v>
@@ -20649,7 +20658,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>18</v>
@@ -20692,7 +20701,7 @@
         <v>56.44</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F7" s="15">
         <v>50.41</v>
@@ -20727,7 +20736,7 @@
         <v>51</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>52</v>
@@ -20953,8 +20962,8 @@
       <c r="J14" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="K14" s="15" t="s">
-        <v>121</v>
+      <c r="K14" s="58" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1">
@@ -20962,34 +20971,34 @@
         <v>12</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E15" s="26" t="s">
         <v>70</v>
       </c>
       <c r="F15" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="H15" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="I15" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="J15" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="K15" s="21" t="s">
         <v>129</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="K15" s="21" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12.75">
@@ -21003,31 +21012,31 @@
         <v>35</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E16" s="26" t="s">
         <v>37</v>
       </c>
       <c r="F16" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="G16" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="H16" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="I16" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="J16" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="K16" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="K16" s="21" t="s">
-        <v>140</v>
-      </c>
       <c r="L16" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
@@ -21035,31 +21044,31 @@
         <v>14</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F17" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="G17" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="H17" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="I17" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="J17" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="K17" s="21" t="s">
         <v>152</v>
-      </c>
-      <c r="K17" s="21" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
@@ -21067,7 +21076,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>19</v>
@@ -21079,22 +21088,22 @@
         <v>30</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H18" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="K18" s="21" t="s">
         <v>157</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="K18" s="21" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1">
@@ -21112,22 +21121,22 @@
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G19" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="H19" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="K19" s="21" t="s">
         <v>162</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="I19" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="K19" s="21" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
@@ -21135,7 +21144,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>19</v>
@@ -21147,22 +21156,22 @@
         <v>30</v>
       </c>
       <c r="F20" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="G20" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="H20" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="K20" s="21" t="s">
         <v>170</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="I20" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="K20" s="21" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="12.75">
@@ -21170,7 +21179,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>35</v>
@@ -21179,22 +21188,22 @@
         <v>24</v>
       </c>
       <c r="F21" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="G21" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="H21" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="K21" s="21" t="s">
         <v>174</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="J21" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="K21" s="21" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="12.75">
@@ -28467,8 +28476,10 @@
     <hyperlink ref="K19" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
     <hyperlink ref="K20" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
     <hyperlink ref="K21" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="K14" r:id="rId17" xr:uid="{6D75F72E-0D0B-4E53-9885-FD2FC35AC17F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -28479,8 +28490,8 @@
   </sheetPr>
   <dimension ref="A1:G1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="A3:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -28496,7 +28507,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" s="56" t="s">
         <v>3</v>
@@ -28525,16 +28536,16 @@
         <v>6</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E3" s="49" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="G3" s="51" t="s">
         <v>187</v>
-      </c>
-      <c r="G3" s="51" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="12.75">
@@ -28542,7 +28553,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C4" s="36" t="s">
         <v>18</v>
@@ -28551,10 +28562,10 @@
         <v>25</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="12.75">
@@ -28571,10 +28582,10 @@
         <v>28</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75">
@@ -28582,7 +28593,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C6" s="36" t="s">
         <v>35</v>
@@ -28591,10 +28602,10 @@
         <v>28</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="12.75">
@@ -28602,7 +28613,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C7" s="36" t="s">
         <v>18</v>
@@ -28614,7 +28625,7 @@
         <v>30</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="12.75">
@@ -28631,7 +28642,7 @@
         <v>41</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="12.75">
@@ -28639,7 +28650,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>35</v>
@@ -28648,10 +28659,10 @@
         <v>45</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="12.75">
@@ -28669,7 +28680,7 @@
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="53" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="12.75">
@@ -28687,7 +28698,7 @@
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="12.75">
@@ -33655,5 +33666,6 @@
     <hyperlink ref="F11" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>